<commit_message>
reverting back to 9-piece objective
</commit_message>
<xml_diff>
--- a/models/siamese_network/models_to_run_checklist.xlsx
+++ b/models/siamese_network/models_to_run_checklist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="53">
   <si>
     <t>C0</t>
   </si>
@@ -87,13 +87,112 @@
   </si>
   <si>
     <t>M=0.99</t>
+  </si>
+  <si>
+    <t>AVG OF BEST VAL EPOCH PER FOLD</t>
+  </si>
+  <si>
+    <t>AVG OF BEST AVG VAL EPOCH</t>
+  </si>
+  <si>
+    <t>0.935/0.786/0.817</t>
+  </si>
+  <si>
+    <t>0.917/0.795/0.805</t>
+  </si>
+  <si>
+    <t>0.938/0.797/0.819</t>
+  </si>
+  <si>
+    <t>0.904/0.786/0.822</t>
+  </si>
+  <si>
+    <t>0.932/0.789/0.817</t>
+  </si>
+  <si>
+    <t>0.944/0.780/0.823</t>
+  </si>
+  <si>
+    <t>0.806/0.794/0.774</t>
+  </si>
+  <si>
+    <t>0.777/0.773/0.789</t>
+  </si>
+  <si>
+    <t>0.837/0.782/0.798</t>
+  </si>
+  <si>
+    <t>0.845/0.770/0.801</t>
+  </si>
+  <si>
+    <t>0.784/0.788/0.802</t>
+  </si>
+  <si>
+    <t>0.792/0.772/0.791</t>
+  </si>
+  <si>
+    <t>0.890/0.799/0.792</t>
+  </si>
+  <si>
+    <t>0.940/0.788/0.784</t>
+  </si>
+  <si>
+    <t>0.960/0.803/0.784</t>
+  </si>
+  <si>
+    <t>0.994/0.792/0.754</t>
+  </si>
+  <si>
+    <t>0.935/0.797/0.798</t>
+  </si>
+  <si>
+    <t>0.971/0.788/0.787</t>
+  </si>
+  <si>
+    <t>0.642/0.655/0.645</t>
+  </si>
+  <si>
+    <t>0.657/0.622/0.642</t>
+  </si>
+  <si>
+    <t>0.669/0.678/0.613</t>
+  </si>
+  <si>
+    <t>0.662/0.643/0.601</t>
+  </si>
+  <si>
+    <t>0.702/0.722/0.729</t>
+  </si>
+  <si>
+    <t>0.717/0.703/0.733</t>
+  </si>
+  <si>
+    <t>0.940/0.789/0.819</t>
+  </si>
+  <si>
+    <t>0.954/0.772/0.823</t>
+  </si>
+  <si>
+    <t>0.910/0.795/0.812</t>
+  </si>
+  <si>
+    <t>0.877/0.779/0.802</t>
+  </si>
+  <si>
+    <t>0.935/0.796/0.821</t>
+  </si>
+  <si>
+    <t>0.955/0.780/0.819</t>
+  </si>
+  <si>
+    <t>TRAIN/VAL/TEST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -120,8 +219,36 @@
       <name val="Avenir Medium"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Avenir Medium"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Avenir Medium"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +291,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD7F8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC4CAFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF301FFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -174,10 +319,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -190,23 +343,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
+      <color rgb="FF301FFF"/>
+      <color rgb="FFFF2EFF"/>
+      <color rgb="FFFFD7F8"/>
+      <color rgb="FFC4CAFF"/>
       <color rgb="FFFFD579"/>
       <color rgb="FFFFB5FE"/>
       <color rgb="FFC8F5FF"/>
       <color rgb="FFDAFFC6"/>
       <color rgb="FFB2C89E"/>
       <color rgb="FFAAEBFF"/>
-      <color rgb="FFC6FFA2"/>
-      <color rgb="FFFFBCAC"/>
-      <color rgb="FFFFFFAA"/>
     </mruColors>
   </colors>
   <extLst>
@@ -480,27 +648,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W58"/>
+  <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="4" width="3.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="8" width="3.6640625" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" customWidth="1"/>
-    <col min="10" max="12" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" customWidth="1"/>
+    <col min="3" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" customWidth="1"/>
+    <col min="11" max="13" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="8"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -518,10 +687,11 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
-    </row>
-    <row r="2" spans="1:23" ht="17" x14ac:dyDescent="0.25">
+      <c r="T1" s="2"/>
+    </row>
+    <row r="2" spans="1:24" ht="17" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="B2" s="8"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -539,12 +709,13 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
-    </row>
-    <row r="3" spans="1:23" ht="17" x14ac:dyDescent="0.25">
+      <c r="T2" s="2"/>
+    </row>
+    <row r="3" spans="1:24" ht="17" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -562,33 +733,34 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
-    </row>
-    <row r="4" spans="1:23" ht="17" x14ac:dyDescent="0.25">
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="1:24" ht="17" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -599,21 +771,22 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
-    </row>
-    <row r="5" spans="1:23" ht="17" x14ac:dyDescent="0.25">
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="1:24" ht="17" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -626,15 +799,16 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
-    </row>
-    <row r="6" spans="1:23" ht="17" x14ac:dyDescent="0.25">
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:24" ht="17" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -651,15 +825,16 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
-    </row>
-    <row r="7" spans="1:23" ht="17" x14ac:dyDescent="0.25">
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:24" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -676,10 +851,11 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
-    </row>
-    <row r="8" spans="1:23" ht="17" x14ac:dyDescent="0.25">
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:24" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
-      <c r="B8" s="2"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -697,11 +873,14 @@
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
-    </row>
-    <row r="9" spans="1:23" ht="17" x14ac:dyDescent="0.25">
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:24" ht="17" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="17" t="s">
+        <v>52</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -718,12 +897,13 @@
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
-    </row>
-    <row r="10" spans="1:23" ht="17" x14ac:dyDescent="0.25">
+      <c r="T9" s="2"/>
+    </row>
+    <row r="10" spans="1:24" ht="17" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -741,43 +921,44 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
-    </row>
-    <row r="11" spans="1:23" ht="17" x14ac:dyDescent="0.25">
+      <c r="T10" s="2"/>
+    </row>
+    <row r="11" spans="1:24" ht="17" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="10"/>
+      <c r="G11" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="J11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="M11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
@@ -788,25 +969,26 @@
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
-    </row>
-    <row r="12" spans="1:23" ht="17" x14ac:dyDescent="0.25">
+      <c r="X11" s="2"/>
+    </row>
+    <row r="12" spans="1:24" ht="17" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="10"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10"/>
+      <c r="F12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="8"/>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
-      <c r="M12" s="2"/>
+      <c r="M12" s="10"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
@@ -817,34 +999,43 @@
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
-    </row>
-    <row r="13" spans="1:23" ht="17" x14ac:dyDescent="0.25">
+      <c r="X12" s="2"/>
+    </row>
+    <row r="13" spans="1:24" ht="17" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="2"/>
+      <c r="B13" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>24</v>
+      </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="J13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="O13" s="2"/>
+      <c r="G13" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="M13" s="14" t="s">
+        <v>42</v>
+      </c>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
@@ -853,29 +1044,41 @@
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
-    </row>
-    <row r="14" spans="1:23" ht="17" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="2"/>
+      <c r="X13" s="2"/>
+    </row>
+    <row r="14" spans="1:24" ht="17" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>25</v>
+      </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="8"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
+      <c r="G14" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="M14" s="16" t="s">
+        <v>43</v>
+      </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -884,34 +1087,58 @@
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
-    </row>
-    <row r="15" spans="1:23" ht="17" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
+      <c r="X14" s="2"/>
+    </row>
+    <row r="15" spans="1:24" ht="17" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
-    </row>
-    <row r="16" spans="1:23" ht="17" x14ac:dyDescent="0.25">
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+    </row>
+    <row r="16" spans="1:24" ht="17" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="B16" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>29</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -926,12 +1153,11 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
-    </row>
-    <row r="17" spans="1:19" ht="17" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2"/>
+      <c r="T16" s="2"/>
+    </row>
+    <row r="17" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -949,33 +1175,20 @@
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
-    </row>
-    <row r="18" spans="1:19" ht="17" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I18" s="2"/>
+      <c r="T17" s="2"/>
+    </row>
+    <row r="18" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -986,15 +1199,26 @@
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
-    </row>
-    <row r="19" spans="1:19" ht="17" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="I19" s="2"/>
+      <c r="T18" s="2"/>
+    </row>
+    <row r="19" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -1005,14 +1229,28 @@
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
-    </row>
-    <row r="20" spans="1:19" ht="17" x14ac:dyDescent="0.25">
+      <c r="T19" s="2"/>
+    </row>
+    <row r="20" spans="1:20" ht="17" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -1023,17 +1261,26 @@
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
-    </row>
-    <row r="21" spans="1:19" ht="17" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+      <c r="T20" s="2"/>
+    </row>
+    <row r="21" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -1044,17 +1291,15 @@
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
-    </row>
-    <row r="22" spans="1:19" ht="17" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+      <c r="T21" s="2"/>
+    </row>
+    <row r="22" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="12"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="8"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
@@ -1065,12 +1310,11 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
-    </row>
-    <row r="23" spans="1:19" ht="17" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="2"/>
+      <c r="T22" s="2"/>
+    </row>
+    <row r="23" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="12"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1088,32 +1332,17 @@
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
-    </row>
-    <row r="24" spans="1:19" ht="17" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="T23" s="2"/>
+    </row>
+    <row r="24" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -1125,14 +1354,19 @@
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
-    </row>
-    <row r="25" spans="1:19" ht="17" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
+      <c r="T24" s="2"/>
+    </row>
+    <row r="25" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -1144,14 +1378,34 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
-    </row>
-    <row r="26" spans="1:19" ht="17" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="8"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
+      <c r="T25" s="2"/>
+    </row>
+    <row r="26" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
@@ -1162,17 +1416,20 @@
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
-    </row>
-    <row r="27" spans="1:19" ht="17" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
+      <c r="T26" s="2"/>
+    </row>
+    <row r="27" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="14"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
@@ -1183,17 +1440,18 @@
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
-    </row>
-    <row r="28" spans="1:19" ht="17" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+      <c r="T27" s="2"/>
+    </row>
+    <row r="28" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="B28" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="16"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -1204,18 +1462,14 @@
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
-    </row>
-    <row r="29" spans="1:19" ht="17" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
+      <c r="T28" s="2"/>
+    </row>
+    <row r="29" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="F29" s="8"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
@@ -1227,32 +1481,17 @@
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
-    </row>
-    <row r="30" spans="1:19" ht="17" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="T29" s="2"/>
+    </row>
+    <row r="30" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
@@ -1264,14 +1503,17 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>
-    </row>
-    <row r="31" spans="1:19" ht="17" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
+      <c r="T30" s="2"/>
+    </row>
+    <row r="31" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -1283,12 +1525,16 @@
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
-    </row>
-    <row r="32" spans="1:19" ht="17" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="8"/>
+      <c r="T31" s="2"/>
+    </row>
+    <row r="32" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -1301,10 +1547,13 @@
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
       <c r="S32" s="2"/>
-    </row>
-    <row r="33" spans="1:19" ht="17" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
+      <c r="T32" s="2"/>
+    </row>
+    <row r="33" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="8"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1322,17 +1571,34 @@
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
-    </row>
-    <row r="34" spans="1:19" ht="17" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
+      <c r="T33" s="2"/>
+    </row>
+    <row r="34" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
@@ -1343,17 +1609,16 @@
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
-    </row>
-    <row r="35" spans="1:19" ht="17" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
+      <c r="T34" s="2"/>
+    </row>
+    <row r="35" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
@@ -1364,31 +1629,29 @@
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
       <c r="S35" s="2"/>
-    </row>
-    <row r="36" spans="1:19" ht="17" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
+      <c r="T35" s="2"/>
+    </row>
+    <row r="36" spans="1:20" ht="17" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="F36" s="8"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-      <c r="Q36" s="2"/>
-      <c r="R36" s="2"/>
-      <c r="S36" s="2"/>
-    </row>
-    <row r="37" spans="1:19" ht="17" x14ac:dyDescent="0.25">
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+    </row>
+    <row r="37" spans="1:20" ht="17" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1396,39 +1659,39 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
-      <c r="Q37" s="2"/>
-      <c r="R37" s="2"/>
-      <c r="S37" s="2"/>
-    </row>
-    <row r="38" spans="1:19" ht="17" x14ac:dyDescent="0.25">
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
-      <c r="Q38" s="2"/>
-      <c r="R38" s="2"/>
-      <c r="S38" s="2"/>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1447,8 +1710,9 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S39" s="1"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1467,8 +1731,9 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S40" s="1"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1487,8 +1752,9 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S41" s="1"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1507,8 +1773,9 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S42" s="1"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1527,8 +1794,9 @@
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S43" s="1"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1547,8 +1815,9 @@
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S44" s="1"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1567,8 +1836,9 @@
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S45" s="1"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1587,8 +1857,9 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S46" s="1"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1607,8 +1878,9 @@
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="S47" s="1"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1627,8 +1899,9 @@
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S48" s="1"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1647,8 +1920,9 @@
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S49" s="1"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1667,8 +1941,9 @@
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S50" s="1"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1687,8 +1962,9 @@
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S51" s="1"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1707,8 +1983,9 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S52" s="1"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1727,8 +2004,9 @@
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S53" s="1"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1747,10 +2025,9 @@
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
+      <c r="S54" s="1"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -1767,65 +2044,7 @@
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
-      <c r="P56" s="1"/>
-      <c r="Q56" s="1"/>
-      <c r="R56" s="1"/>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
-      <c r="K57" s="1"/>
-      <c r="L57" s="1"/>
-      <c r="M57" s="1"/>
-      <c r="N57" s="1"/>
-      <c r="O57" s="1"/>
-      <c r="P57" s="1"/>
-      <c r="Q57" s="1"/>
-      <c r="R57" s="1"/>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
-      <c r="O58" s="1"/>
-      <c r="P58" s="1"/>
-      <c r="Q58" s="1"/>
-      <c r="R58" s="1"/>
+      <c r="S55" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>